<commit_message>
Aggiunto Sophie Lv4 vs Captain.
</commit_message>
<xml_diff>
--- a/Documents/LevelDesignDocument/Images/Exp chart.xlsx
+++ b/Documents/LevelDesignDocument/Images/Exp chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Varie\Team delle Lande\teamdellelande\Documents\LevelDesignDocument\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD6BE34-4228-434F-B801-A7CE04BCDE59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB39E2C8-B050-4004-B2C7-6F6F694E99B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>Exp</t>
   </si>
@@ -116,13 +116,19 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>Fight/Avoid demons in streets</t>
+  </si>
+  <si>
+    <t>Avoid/Defeat all enemies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +138,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -229,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -244,6 +258,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -739,8 +755,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AB0AD90-F8B8-4427-813D-D15561BF102A}" name="Tabella135" displayName="Tabella135" ref="A11:G30" totalsRowShown="0" tableBorderDxfId="4">
-  <autoFilter ref="A11:G30" xr:uid="{1C1C74C2-6A9E-4539-B9A5-0D523F81F50F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AB0AD90-F8B8-4427-813D-D15561BF102A}" name="Tabella135" displayName="Tabella135" ref="A11:G31" totalsRowShown="0" tableBorderDxfId="4">
+  <autoFilter ref="A11:G31" xr:uid="{1C1C74C2-6A9E-4539-B9A5-0D523F81F50F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{3E497371-C991-4D9E-B61B-09CA22A5D62C}" name="Activity"/>
     <tableColumn id="3" xr3:uid="{2C851A9A-62BE-4069-B4E0-CEC0B082F3E5}" name="Exp"/>
@@ -1995,15 +2011,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32A71DCF-E2A2-4A9E-AE5D-65E7B4554532}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -2359,28 +2375,28 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="12">
         <v>3250</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="12">
         <v>250</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="12">
         <f>Tabella135[[#This Row],[Exp]]</f>
         <v>3250</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="13">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
         <v>3</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="12">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]</f>
         <v>3500</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="12">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
         <v>3</v>
       </c>
@@ -2462,15 +2478,14 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3">
-        <v>150</v>
+        <v>30</v>
+      </c>
+      <c r="B16" s="3">
+        <v>100</v>
       </c>
       <c r="D16" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D15</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E16" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2478,7 +2493,7 @@
       </c>
       <c r="F16" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F15</f>
-        <v>3800</v>
+        <v>3750</v>
       </c>
       <c r="G16" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2487,7 +2502,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3">
@@ -2495,7 +2510,7 @@
       </c>
       <c r="D17" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D16</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E17" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2503,7 +2518,7 @@
       </c>
       <c r="F17" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F16</f>
-        <v>3950</v>
+        <v>3900</v>
       </c>
       <c r="G17" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2512,7 +2527,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3">
@@ -2520,7 +2535,7 @@
       </c>
       <c r="D18" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D17</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E18" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2528,7 +2543,7 @@
       </c>
       <c r="F18" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F17</f>
-        <v>4100</v>
+        <v>4050</v>
       </c>
       <c r="G18" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2537,7 +2552,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3">
@@ -2545,7 +2560,7 @@
       </c>
       <c r="D19" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D18</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E19" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2553,7 +2568,7 @@
       </c>
       <c r="F19" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F18</f>
-        <v>4250</v>
+        <v>4200</v>
       </c>
       <c r="G19" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2562,7 +2577,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3">
@@ -2570,7 +2585,7 @@
       </c>
       <c r="D20" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D19</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E20" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2578,7 +2593,7 @@
       </c>
       <c r="F20" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F19</f>
-        <v>4400</v>
+        <v>4350</v>
       </c>
       <c r="G20" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2587,7 +2602,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3">
@@ -2595,7 +2610,7 @@
       </c>
       <c r="D21" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D20</f>
-        <v>3400</v>
+        <v>3500</v>
       </c>
       <c r="E21" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2603,7 +2618,7 @@
       </c>
       <c r="F21" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F20</f>
-        <v>4550</v>
+        <v>4500</v>
       </c>
       <c r="G21" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2612,15 +2627,15 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="3">
-        <v>200</v>
-      </c>
-      <c r="C22" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3">
+        <v>150</v>
+      </c>
       <c r="D22" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D21</f>
-        <v>3600</v>
+        <v>3500</v>
       </c>
       <c r="E22" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2628,7 +2643,7 @@
       </c>
       <c r="F22" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F21</f>
-        <v>4750</v>
+        <v>4650</v>
       </c>
       <c r="G22" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2637,15 +2652,15 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D22</f>
-        <v>3800</v>
+        <v>3600</v>
       </c>
       <c r="E23" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2653,7 +2668,7 @@
       </c>
       <c r="F23" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F22</f>
-        <v>4950</v>
+        <v>4750</v>
       </c>
       <c r="G23" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2662,15 +2677,15 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D23</f>
-        <v>4000</v>
+        <v>3725</v>
       </c>
       <c r="E24" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2678,7 +2693,7 @@
       </c>
       <c r="F24" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F23</f>
-        <v>5150</v>
+        <v>4875</v>
       </c>
       <c r="G24" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2687,15 +2702,15 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="3">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D24</f>
-        <v>4200</v>
+        <v>3875</v>
       </c>
       <c r="E25" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2703,7 +2718,7 @@
       </c>
       <c r="F25" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F24</f>
-        <v>5350</v>
+        <v>5025</v>
       </c>
       <c r="G25" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2712,15 +2727,15 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3">
-        <v>600</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B26" s="3">
+        <v>225</v>
+      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D25</f>
-        <v>4200</v>
+        <v>4100</v>
       </c>
       <c r="E26" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2728,24 +2743,24 @@
       </c>
       <c r="F26" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F25</f>
-        <v>5950</v>
+        <v>5250</v>
       </c>
       <c r="G26" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="3">
-        <v>700</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3">
+        <v>500</v>
+      </c>
       <c r="D27" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D26</f>
-        <v>4900</v>
+        <v>4100</v>
       </c>
       <c r="E27" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2753,7 +2768,7 @@
       </c>
       <c r="F27" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F26</f>
-        <v>6650</v>
+        <v>5750</v>
       </c>
       <c r="G27" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2762,15 +2777,15 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3">
-        <v>250</v>
+        <v>700</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D27</f>
-        <v>5150</v>
+        <v>4800</v>
       </c>
       <c r="E28" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2778,32 +2793,32 @@
       </c>
       <c r="F28" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F27</f>
-        <v>6900</v>
+        <v>6450</v>
       </c>
       <c r="G28" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3">
-        <v>900</v>
+        <v>250</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D28</f>
-        <v>6050</v>
+        <v>5050</v>
       </c>
       <c r="E29" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F28</f>
-        <v>7800</v>
+        <v>6700</v>
       </c>
       <c r="G29" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2811,25 +2826,50 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="3">
+        <v>900</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <f>Tabella135[[#This Row],[Exp]]+D29</f>
+        <v>5950</v>
+      </c>
+      <c r="E30" s="4">
+        <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
+        <v>4</v>
+      </c>
+      <c r="F30" s="3">
+        <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F29</f>
+        <v>7600</v>
+      </c>
+      <c r="G30" s="4">
+        <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
-        <f>SUM(B13:B29)</f>
-        <v>2800</v>
-      </c>
-      <c r="C30" s="1">
-        <f>SUM(C13:C29)</f>
-        <v>1500</v>
-      </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
+      <c r="B31" s="1">
+        <f>SUM(B13:B30)</f>
+        <v>2700</v>
+      </c>
+      <c r="C31" s="1">
+        <f>SUM(C13:C30)</f>
+        <v>1400</v>
+      </c>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E8">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2843,7 +2883,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G8">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2856,8 +2896,36 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E29">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="E12">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{569B6A1E-9469-4A01-A346-FB64CF4496A6}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E8 G2:G8">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{931E836D-501D-4976-AF7C-B42E033D3259}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13:E30">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2870,8 +2938,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12:G30">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="G12:G31">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2884,22 +2952,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{569B6A1E-9469-4A01-A346-FB64CF4496A6}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E30">
-    <cfRule type="dataBar" priority="5">
+  <conditionalFormatting sqref="E12:E31">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2912,7 +2966,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E8 G2:G8">
+  <conditionalFormatting sqref="E12:E30 G12:G30">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -2921,7 +2975,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{931E836D-501D-4976-AF7C-B42E033D3259}</x14:id>
+          <x14:id>{9CC17562-523A-442E-A77F-AC51970BF46E}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2958,28 +3012,6 @@
           <xm:sqref>G2:G8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{73E65424-1607-45BA-B247-0BCD1E8B337C}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E13:E29</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1C400EA7-A2C6-4B22-9AD7-9E2D09BF507A}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G12:G30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{569B6A1E-9469-4A01-A346-FB64CF4496A6}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="autoMin"/>
@@ -2989,17 +3021,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>E12</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FD2BC0FA-1EB2-4848-B05F-9F83AD1AB03F}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E12:E30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{931E836D-501D-4976-AF7C-B42E033D3259}">
@@ -3012,6 +3033,50 @@
           </x14:cfRule>
           <xm:sqref>E2:E8 G2:G8</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{73E65424-1607-45BA-B247-0BCD1E8B337C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E13:E30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1C400EA7-A2C6-4B22-9AD7-9E2D09BF507A}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G12:G31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FD2BC0FA-1EB2-4848-B05F-9F83AD1AB03F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E12:E31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9CC17562-523A-442E-A77F-AC51970BF46E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E12:E30 G12:G30</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Aggiunte posizione nemici, aggiornata tabella exp.
</commit_message>
<xml_diff>
--- a/Documents/LevelDesignDocument/Images/Exp chart.xlsx
+++ b/Documents/LevelDesignDocument/Images/Exp chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Varie\Team delle Lande\teamdellelande\Documents\LevelDesignDocument\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB39E2C8-B050-4004-B2C7-6F6F694E99B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06479B-54B4-4AF6-A78E-A9D2DD25D13C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2014,7 +2014,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="F13" sqref="F13:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,11 +2481,11 @@
         <v>30</v>
       </c>
       <c r="B16" s="3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D16" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D15</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E16" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="F16" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F15</f>
-        <v>3750</v>
+        <v>3850</v>
       </c>
       <c r="G16" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="D17" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D16</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E17" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="F17" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F16</f>
-        <v>3900</v>
+        <v>4000</v>
       </c>
       <c r="G17" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2535,7 +2535,7 @@
       </c>
       <c r="D18" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D17</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E18" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="F18" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F17</f>
-        <v>4050</v>
+        <v>4150</v>
       </c>
       <c r="G18" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2560,7 +2560,7 @@
       </c>
       <c r="D19" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D18</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E19" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="F19" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F18</f>
-        <v>4200</v>
+        <v>4300</v>
       </c>
       <c r="G19" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="D20" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D19</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E20" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="F20" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F19</f>
-        <v>4350</v>
+        <v>4450</v>
       </c>
       <c r="G20" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="D21" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D20</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E21" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="F21" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F20</f>
-        <v>4500</v>
+        <v>4600</v>
       </c>
       <c r="G21" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2635,7 +2635,7 @@
       </c>
       <c r="D22" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D21</f>
-        <v>3500</v>
+        <v>3600</v>
       </c>
       <c r="E22" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="F22" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F21</f>
-        <v>4650</v>
+        <v>4750</v>
       </c>
       <c r="G22" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2660,7 +2660,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D22</f>
-        <v>3600</v>
+        <v>3700</v>
       </c>
       <c r="E23" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="F23" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F22</f>
-        <v>4750</v>
+        <v>4850</v>
       </c>
       <c r="G23" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2680,12 +2680,12 @@
         <v>16</v>
       </c>
       <c r="B24" s="3">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D23</f>
-        <v>3725</v>
+        <v>3850</v>
       </c>
       <c r="E24" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2693,7 +2693,7 @@
       </c>
       <c r="F24" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F23</f>
-        <v>4875</v>
+        <v>5000</v>
       </c>
       <c r="G24" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2705,12 +2705,12 @@
         <v>17</v>
       </c>
       <c r="B25" s="3">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D24</f>
-        <v>3875</v>
+        <v>4050</v>
       </c>
       <c r="E25" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="F25" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F24</f>
-        <v>5025</v>
+        <v>5200</v>
       </c>
       <c r="G25" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2730,12 +2730,12 @@
         <v>18</v>
       </c>
       <c r="B26" s="3">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D25</f>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="E26" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="F26" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F25</f>
-        <v>5250</v>
+        <v>5450</v>
       </c>
       <c r="G26" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2756,11 +2756,11 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="D27" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D26</f>
-        <v>4100</v>
+        <v>4300</v>
       </c>
       <c r="E27" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2768,7 +2768,7 @@
       </c>
       <c r="F27" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F26</f>
-        <v>5750</v>
+        <v>6050</v>
       </c>
       <c r="G27" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2780,12 +2780,12 @@
         <v>19</v>
       </c>
       <c r="B28" s="3">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D27</f>
-        <v>4800</v>
+        <v>4900</v>
       </c>
       <c r="E28" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="F28" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F27</f>
-        <v>6450</v>
+        <v>6650</v>
       </c>
       <c r="G28" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2810,7 +2810,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D28</f>
-        <v>5050</v>
+        <v>5150</v>
       </c>
       <c r="E29" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2818,7 +2818,7 @@
       </c>
       <c r="F29" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F28</f>
-        <v>6700</v>
+        <v>6900</v>
       </c>
       <c r="G29" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2835,7 +2835,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D29</f>
-        <v>5950</v>
+        <v>6050</v>
       </c>
       <c r="E30" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="F30" s="3">
         <f>Tabella135[[#This Row],[Exp]]+Tabella135[[#This Row],[Exp opt]]+F29</f>
-        <v>7600</v>
+        <v>7800</v>
       </c>
       <c r="G30" s="4">
         <f>IF(Tabella135[[#This Row],[Sum max]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum max]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum max]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum max]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum max]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum max]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum max]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum max]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2856,11 +2856,11 @@
       </c>
       <c r="B31" s="1">
         <f>SUM(B13:B30)</f>
-        <v>2700</v>
+        <v>2800</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C13:C30)</f>
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>

</xml_diff>

<commit_message>
Ri-aggiornate tabelle exp, aggiunta missione secondaria Evita i quattro demoni in città.
</commit_message>
<xml_diff>
--- a/Documents/LevelDesignDocument/Images/Exp chart.xlsx
+++ b/Documents/LevelDesignDocument/Images/Exp chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Varie\Team delle Lande\teamdellelande\Documents\LevelDesignDocument\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B06479B-54B4-4AF6-A78E-A9D2DD25D13C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58132CFD-3B28-470F-B285-8F33C1305463}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2014,7 +2014,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F30"/>
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,14 +2136,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="7">
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="C4" s="7">
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="D4" s="7">
         <f>Tabella14[[#This Row],[Exp]]+D3</f>
-        <v>6050</v>
+        <v>5850</v>
       </c>
       <c r="E4" s="7">
         <f>IF(Tabella14[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella14[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella14[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella14[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella14[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella14[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella14[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella14[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="D5" s="7">
         <f>Tabella14[[#This Row],[Exp]]+D4</f>
-        <v>10250</v>
+        <v>10050</v>
       </c>
       <c r="E5" s="7">
         <f>IF(Tabella14[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella14[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella14[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella14[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella14[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella14[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella14[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella14[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="D6" s="7">
         <f>Tabella14[[#This Row],[Exp]]+D5</f>
-        <v>17050</v>
+        <v>16850</v>
       </c>
       <c r="E6" s="7">
         <f>IF(Tabella14[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella14[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella14[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella14[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella14[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella14[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella14[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella14[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="D7" s="7">
         <f>Tabella14[[#This Row],[Exp]]+D6</f>
-        <v>25650</v>
+        <v>25450</v>
       </c>
       <c r="E7" s="7">
         <f>IF(Tabella14[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella14[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella14[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella14[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella14[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella14[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella14[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella14[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D8" s="7">
         <f>Tabella14[[#This Row],[Exp]]+D7</f>
-        <v>35350</v>
+        <v>35150</v>
       </c>
       <c r="E8" s="7">
         <f>IF(Tabella14[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella14[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella14[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella14[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella14[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella14[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella14[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella14[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2480,12 +2480,13 @@
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="3"/>
+      <c r="C16">
         <v>200</v>
       </c>
       <c r="D16" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D15</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E16" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2510,7 +2511,7 @@
       </c>
       <c r="D17" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D16</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E17" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2535,7 +2536,7 @@
       </c>
       <c r="D18" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D17</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E18" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2560,7 +2561,7 @@
       </c>
       <c r="D19" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D18</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E19" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2585,7 +2586,7 @@
       </c>
       <c r="D20" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D19</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E20" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2610,7 +2611,7 @@
       </c>
       <c r="D21" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D20</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E21" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2635,7 +2636,7 @@
       </c>
       <c r="D22" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D21</f>
-        <v>3600</v>
+        <v>3400</v>
       </c>
       <c r="E22" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2660,7 +2661,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D22</f>
-        <v>3700</v>
+        <v>3500</v>
       </c>
       <c r="E23" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2685,7 +2686,7 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D23</f>
-        <v>3850</v>
+        <v>3650</v>
       </c>
       <c r="E24" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2710,7 +2711,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D24</f>
-        <v>4050</v>
+        <v>3850</v>
       </c>
       <c r="E25" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2735,7 +2736,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D25</f>
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="E26" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2760,7 +2761,7 @@
       </c>
       <c r="D27" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D26</f>
-        <v>4300</v>
+        <v>4100</v>
       </c>
       <c r="E27" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2785,7 +2786,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D27</f>
-        <v>4900</v>
+        <v>4700</v>
       </c>
       <c r="E28" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2810,7 +2811,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D28</f>
-        <v>5150</v>
+        <v>4950</v>
       </c>
       <c r="E29" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2835,7 +2836,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3">
         <f>Tabella135[[#This Row],[Exp]]+D29</f>
-        <v>6050</v>
+        <v>5850</v>
       </c>
       <c r="E30" s="4">
         <f>IF(Tabella135[[#This Row],[Sum min]]&gt;J$11,I$11,IF(Tabella135[[#This Row],[Sum min]]&gt;J$10,I$10,IF(Tabella135[[#This Row],[Sum min]]&gt;J$9,I$9,IF(Tabella135[[#This Row],[Sum min]]&gt;J$8,I$8,IF(Tabella135[[#This Row],[Sum min]]&gt;J$7,I$7,IF(Tabella135[[#This Row],[Sum min]]&gt;J$6,I$6,IF(Tabella135[[#This Row],[Sum min]]&gt;J$5,I$5,IF(Tabella135[[#This Row],[Sum min]]&gt;J$4,I$4,I$3))))))))</f>
@@ -2856,11 +2857,11 @@
       </c>
       <c r="B31" s="1">
         <f>SUM(B13:B30)</f>
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="C31" s="1">
         <f>SUM(C13:C30)</f>
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10"/>

</xml_diff>